<commit_message>
Agrega nuevos archivos en actualizacion de descarga de archivos
</commit_message>
<xml_diff>
--- a/build/assets/statics/bdb/REEXPEDICION.xlsx
+++ b/build/assets/statics/bdb/REEXPEDICION.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25128"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\squijano\Desktop\BANCO DE BOGOTA\ARCHIVOS AUTOGESTION CEO\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2262F2C7-D07F-4513-A138-D0B21170F790}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB6BEDAC-026D-4948-BC2D-A2DF276F8585}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="473" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -381,7 +381,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="12">
+  <borders count="14">
     <border>
       <left/>
       <right/>
@@ -538,13 +538,43 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color theme="0" tint="-0.14996795556505021"/>
+      </left>
+      <right style="thin">
+        <color theme="0" tint="-0.14993743705557422"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color theme="0" tint="-0.14996795556505021"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0" tint="-0.14996795556505021"/>
+      </left>
+      <right style="thin">
+        <color theme="0" tint="-0.14996795556505021"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color theme="0" tint="-0.14996795556505021"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="52">
+  <cellXfs count="54">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyProtection="1">
       <protection locked="0"/>
@@ -691,6 +721,12 @@
     </xf>
     <xf numFmtId="49" fontId="8" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -1263,11 +1299,10 @@
   <cols>
     <col min="1" max="1" width="14.88671875" style="1" customWidth="1"/>
     <col min="2" max="2" width="20.33203125" style="2" customWidth="1"/>
-    <col min="3" max="3" width="19.109375" style="2" customWidth="1"/>
-    <col min="4" max="4" width="21.33203125" style="2" customWidth="1"/>
-    <col min="5" max="5" width="21.44140625" style="3" customWidth="1"/>
-    <col min="6" max="6" width="17.88671875" style="3" customWidth="1"/>
-    <col min="7" max="7" width="10.88671875" style="4" customWidth="1"/>
+    <col min="3" max="4" width="22.21875" style="2" customWidth="1"/>
+    <col min="5" max="5" width="21.21875" style="3" customWidth="1"/>
+    <col min="6" max="6" width="21.44140625" style="3" customWidth="1"/>
+    <col min="7" max="7" width="12.5546875" style="4" customWidth="1"/>
     <col min="8" max="8" width="19" style="5" customWidth="1"/>
     <col min="9" max="9" width="12.88671875" style="4" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="9.88671875" style="4" customWidth="1"/>
@@ -1512,12 +1547,12 @@
       <c r="Q10" s="35"/>
     </row>
     <row r="11" spans="1:17" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="3"/>
-      <c r="B11" s="3"/>
-      <c r="C11" s="3"/>
-      <c r="D11" s="3"/>
-      <c r="E11" s="3"/>
-      <c r="F11" s="3"/>
+      <c r="A11" s="53"/>
+      <c r="B11" s="53"/>
+      <c r="C11" s="53"/>
+      <c r="D11" s="53"/>
+      <c r="E11" s="53"/>
+      <c r="F11" s="52"/>
       <c r="G11" s="43"/>
       <c r="H11" s="13"/>
       <c r="I11" s="13"/>
@@ -6262,7 +6297,7 @@
       <c r="G510" s="12"/>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="bLxjGmJjUR6rxaoKjWGtkizfoeXg6SymTm7ikIIMWDXKQeBbE2A3oRbJcC6fR0scNIvnMxa5RyXkRh1vE9LcgA==" saltValue="0JCyEZMnS2FqbaeIsYUt6Q==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="3zr9ujveWKAKtXMhZxnb1XaSEgd34aTLZVZb3aoZ2oNEULmoiJRMDbN4r7Y6o7H6TjRH//lnxflbRpA1t/n3Gw==" saltValue="f7H3fZpBqEBdO6r9b8QYyQ==" spinCount="100000" sheet="1" objects="1" scenarios="1" formatCells="0" formatColumns="0"/>
   <protectedRanges>
     <protectedRange sqref="H10:N35 A11:F510" name="Rango1_1"/>
     <protectedRange sqref="A8:D8" name="Rango1_1_1_1"/>

</xml_diff>